<commit_message>
Made changes for cross-billing.
</commit_message>
<xml_diff>
--- a/Data Requests and Statuses.xlsx
+++ b/Data Requests and Statuses.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>System</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Customer Data</t>
   </si>
   <si>
-    <t>A format for all the purchase of tokens in the last 24 months</t>
-  </si>
-  <si>
     <t>Deposit Format</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>There is need to map current Bairros and streets in the Cadastramento to the correct CSC</t>
   </si>
   <si>
-    <t>To be discussed in the meeting</t>
-  </si>
-  <si>
     <t>Employee IDs</t>
   </si>
   <si>
@@ -150,12 +144,6 @@
     <t>No communication from EDM on the status</t>
   </si>
   <si>
-    <t>EDM preparing sample extraction</t>
-  </si>
-  <si>
-    <t>We have not received billing formats for Access and this can wait until we finish billing first.</t>
-  </si>
-  <si>
     <t>EDM to provide data</t>
   </si>
   <si>
@@ -169,6 +157,27 @@
   </si>
   <si>
     <t>Format ready and sent to EDM.</t>
+  </si>
+  <si>
+    <t>A format for all the purchase of tokens in the last 24 months. Also to add a record for the unpaid bill amount in Eclipse.</t>
+  </si>
+  <si>
+    <t>EDM sent us a file with the mapping however the data does not correspond to Cadastramento. We asked EDM to match the Cadastramento data.</t>
+  </si>
+  <si>
+    <t>Will be required for go-live</t>
+  </si>
+  <si>
+    <t>Sample extractions were provided by EDM</t>
+  </si>
+  <si>
+    <t>This is not clear whether we will use NUIT, National ID no. or Employee no.</t>
+  </si>
+  <si>
+    <t>Further consultations required on the split formula</t>
+  </si>
+  <si>
+    <t>Further consultations required on this</t>
   </si>
 </sst>
 </file>
@@ -560,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -589,13 +598,13 @@
         <v>3</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="51.75">
@@ -612,13 +621,13 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="3">
         <v>41585</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="26.25">
@@ -635,13 +644,13 @@
         <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="7">
         <v>41578</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="102.75">
@@ -655,16 +664,16 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
         <v>41584</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="26.25">
@@ -681,16 +690,16 @@
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="3">
         <v>41584</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="26.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="39">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -698,19 +707,19 @@
         <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="9">
         <v>41585</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:8">
@@ -718,45 +727,45 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G8" s="9">
         <v>41593</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="51.75">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="26.25">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G9" s="9">
         <v>41593</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="26.25">
@@ -764,147 +773,157 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="10">
         <v>41591</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="26.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="77.25">
       <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="39">
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="2:8" ht="26.25">
-      <c r="B12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="E12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="39">
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="39">
       <c r="B14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="2:8" ht="26.25">
-      <c r="B15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="2:8" ht="26.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="10">
-        <v>41600</v>
+        <v>20</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="H16" s="1"/>
     </row>

</xml_diff>